<commit_message>
Added extent report and Logger
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -1,17 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4BC9A570-8276-4315-8A07-7DCED4264061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{73FFE2CA-674C-4D01-9469-8CF6A1F1A838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OrangeHRMTest" sheetId="13" r:id="rId1"/>
+    <sheet name="OrangeHRMLeaves" sheetId="14" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="15" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <oleSize ref="A3:K23"/>
+  <oleSize ref="A1:K7"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="34">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -117,6 +119,18 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>OrangeHRM Login Test</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Admin1223</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -524,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42C0D6C-0871-4C9E-8F75-08F6F35C1FB7}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,7 +562,7 @@
     <col min="16" max="16" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -583,7 +597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -607,7 +621,7 @@
       </c>
       <c r="H2" s="3" t="str">
         <f ca="1">_xlfn.CONCAT("User-", TEXT(NOW(), "ddmmyyyyhhmmss"), RANDBETWEEN(1,100))</f>
-        <v>User-3101202608423217</v>
+        <v>User-1502202611204522</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>20</v>
@@ -619,7 +633,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -645,7 +659,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -671,7 +685,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -697,7 +711,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -715,7 +729,7 @@
       </c>
       <c r="F6" s="3" t="str">
         <f ca="1">_xlfn.CONCAT("Shift-", TEXT(NOW(), "ddmmyyyyhhmmss"))</f>
-        <v>Shift-31012026084232</v>
+        <v>Shift-15022026112045</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>25</v>
@@ -724,9 +738,68 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:11" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:11" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:11" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>4</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>4</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+    </row>
+    <row r="10" spans="1:13" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:13" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:13" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:13" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" xr:uid="{55BF875E-FA4A-44D6-92D4-797217977042}"/>
@@ -734,4 +807,65 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F792A868-2585-4740-A0B2-13BEE7D51DD0}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67EA428-0523-4517-AE4C-3F303F4B2AA9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>